<commit_message>
something weird is happening
</commit_message>
<xml_diff>
--- a/static/copilotstatic/scraped_info.xlsx
+++ b/static/copilotstatic/scraped_info.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>45303.773249454</v>
+        <v>45303.77324945602</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -2676,6 +2676,126 @@
       <c r="D112" t="inlineStr">
         <is>
           <t>12,122,594</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>45308.01676148148</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>505 Ratings</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>(5,777,119 Downloads)</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>12,235,109</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>45309.01675581018</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>506 Ratings</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>(5,798,182 Downloads)</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>12,271,244</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>45310.01675893518</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>509 Ratings</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>(5,817,928 Downloads)</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>12,309,040</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45311.01675642361</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>513 Ratings</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>(5,837,262 Downloads)</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>12,342,069</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>45312.01675711806</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>513 Ratings</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>(5,855,553 Downloads)</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>12,361,900</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>45313.01675682763</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>513 Ratings</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>(5,864,546 Downloads)</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>12,380,933</t>
         </is>
       </c>
     </row>

</xml_diff>